<commit_message>
Padam Input Raja changes in GM 06/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Restriction on Sandhi Rules.xlsx
+++ b/TS Jatai Working/Raja Files/Restriction on Sandhi Rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Vowel Sandhi</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">Apo + vai becomes Apo vA </t>
   </si>
   <si>
-    <t>Letter</t>
-  </si>
-  <si>
     <t>FW LL</t>
   </si>
   <si>
@@ -88,26 +85,92 @@
     <t>NamO astu</t>
   </si>
   <si>
-    <t>NamaH agriyAya, SaH indra</t>
-  </si>
-  <si>
     <t>Sandhi Alowed on</t>
   </si>
   <si>
-    <t>Special rules in Table                         e.g saH+it =set</t>
-  </si>
-  <si>
     <t>Let us Test few cases with Sandhi Rules, Visargam-drop cases, No Elision Rules with normal sandhi I have given in the end.</t>
   </si>
   <si>
     <t>Note: If there is no application of above rules but a combination of vowels continuously apply Sandhi.</t>
+  </si>
+  <si>
+    <t>Paragraha (PG)</t>
+  </si>
+  <si>
+    <t>PG LL</t>
+  </si>
+  <si>
+    <t>Elision or Sandhi allowed with the FL of PG with previous word                e.g. iti+atho = ityatho</t>
+  </si>
+  <si>
+    <t>Notations:</t>
+  </si>
+  <si>
+    <t>FW</t>
+  </si>
+  <si>
+    <t>First Word</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>Next Word</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>First Letter</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>Last Letter</t>
+  </si>
+  <si>
+    <t>I, e,U,o</t>
+  </si>
+  <si>
+    <t>Word/Letter</t>
+  </si>
+  <si>
+    <t>NamaH agriyAya, SaH indra,              devAH abavann = devA abavann</t>
+  </si>
+  <si>
+    <t>Special rules in Table(indicated in Excel)          e.g saH+it =set</t>
+  </si>
+  <si>
+    <t>Avagraha</t>
+  </si>
+  <si>
+    <t>A,e,o</t>
+  </si>
+  <si>
+    <t>existing or formed due to Sandhi</t>
+  </si>
+  <si>
+    <t>No Further Sandhi</t>
+  </si>
+  <si>
+    <t>Avagraha so no change</t>
+  </si>
+  <si>
+    <t>FW FL , NW LL</t>
+  </si>
+  <si>
+    <t>FW FL, NW LL</t>
+  </si>
+  <si>
+    <t>FW FL,NW LL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,7 +185,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -154,17 +230,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,19 +551,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J267"/>
+  <dimension ref="A1:J268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:G21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.7109375" customWidth="1"/>
@@ -514,26 +595,26 @@
     </row>
     <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>25</v>
+      <c r="H3" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -557,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -566,22 +647,22 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
+      <c r="H6" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -590,10 +671,10 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>10</v>
@@ -630,30 +711,30 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>14</v>
+      <c r="G11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="36" x14ac:dyDescent="0.25">
@@ -663,8 +744,8 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="6" t="s">
-        <v>26</v>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -688,14 +769,24 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:10" ht="54" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -710,28 +801,28 @@
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>14</v>
+      <c r="H17" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
@@ -744,31 +835,45 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+    <row r="19" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -779,13 +884,15 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
@@ -799,9 +906,15 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -810,8 +923,12 @@
     </row>
     <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="B25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -820,8 +937,12 @@
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -830,8 +951,12 @@
     </row>
     <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -3238,6 +3363,16 @@
       <c r="G267" s="1"/>
       <c r="H267" s="1"/>
     </row>
+    <row r="268" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A268" s="1"/>
+      <c r="B268" s="1"/>
+      <c r="C268" s="1"/>
+      <c r="D268" s="1"/>
+      <c r="E268" s="1"/>
+      <c r="F268" s="1"/>
+      <c r="G268" s="1"/>
+      <c r="H268" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>